<commit_message>
Make the app work for both local file and the PostgreSQL
</commit_message>
<xml_diff>
--- a/Geartek.xlsx
+++ b/Geartek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\iviewsense_beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D010F4-002B-45C3-8C44-91B5896FE61E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CA7F9-B951-44B1-ACA8-0D4B08A6CED3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1189,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AN7" sqref="AN7"/>
     </sheetView>
   </sheetViews>

</xml_diff>